<commit_message>
added dummy data to expermint on them
</commit_message>
<xml_diff>
--- a/projects_data.xlsx
+++ b/projects_data.xlsx
@@ -1,57 +1,146 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+  <si>
+    <t>project title</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Total target</t>
+  </si>
+  <si>
+    <t>Start date</t>
+  </si>
+  <si>
+    <t>End date</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>omar</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>first project</t>
+  </si>
+  <si>
+    <t>start funding for school</t>
+  </si>
+  <si>
+    <t>22/7/2010</t>
+  </si>
+  <si>
+    <t>22/8/2010</t>
+  </si>
+  <si>
+    <t>mostafa</t>
+  </si>
+  <si>
+    <t>nour</t>
+  </si>
+  <si>
+    <t>mahmoud</t>
+  </si>
+  <si>
+    <t>22/9/2021</t>
+  </si>
+  <si>
+    <t>22/12/2021</t>
+  </si>
+  <si>
+    <t>30/3/2021</t>
+  </si>
+  <si>
+    <t>crtical surgary</t>
+  </si>
+  <si>
+    <t>new iphone</t>
+  </si>
+  <si>
+    <t>gaming set</t>
+  </si>
+  <si>
+    <t>weekend at hawaii</t>
+  </si>
+  <si>
+    <t>second project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">third project </t>
+  </si>
+  <si>
+    <t>fourth project</t>
+  </si>
+  <si>
+    <t>fifth project</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>abc_cd@ed.com</t>
+  </si>
+  <si>
+    <t>cd_ed@ed.com</t>
+  </si>
+  <si>
+    <t>xyz_as@ed.com</t>
+  </si>
+  <si>
+    <t>af_o@ed.com</t>
+  </si>
+  <si>
+    <t>wtf@ed.com</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="3">
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="1"/>
-      <family val="0"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
+      <u/>
       <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
+      <color theme="10"/>
       <name val="Arial"/>
       <charset val="1"/>
-      <family val="0"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="15"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -63,7 +152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -72,49 +161,68 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -173,6 +281,14 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -462,148 +578,258 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AMK75"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col width="24.6" customWidth="1" style="3" min="1" max="1"/>
-    <col width="48.21" customWidth="1" style="3" min="2" max="2"/>
-    <col width="21.82" customWidth="1" style="3" min="3" max="3"/>
-    <col width="18.77" customWidth="1" style="3" min="4" max="4"/>
-    <col width="21.67" customWidth="1" style="3" min="5" max="5"/>
-    <col width="28.76" customWidth="1" style="3" min="6" max="6"/>
-    <col width="14.43" customWidth="1" style="3" min="7" max="1025"/>
+    <col min="1" max="1" width="24.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" style="1" customWidth="1"/>
+    <col min="7" max="1025" width="14.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="35.25" customHeight="1" s="4">
-      <c r="A1" s="5" t="inlineStr">
-        <is>
-          <t>project title</t>
-        </is>
-      </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t>Details</t>
-        </is>
-      </c>
-      <c r="C1" s="5" t="inlineStr">
-        <is>
-          <t>Total target</t>
-        </is>
-      </c>
-      <c r="D1" s="5" t="inlineStr">
-        <is>
-          <t>Start date</t>
-        </is>
-      </c>
-      <c r="E1" s="5" t="inlineStr">
-        <is>
-          <t>End date</t>
-        </is>
-      </c>
-      <c r="F1" s="5" t="inlineStr">
-        <is>
-          <t>Owner</t>
-        </is>
+    <row r="1" spans="1:8" ht="35.25" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="2" ht="26.25" customHeight="1" s="4">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>w</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>omar</t>
-        </is>
+    <row r="2" spans="1:8" ht="26.25" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2500</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4">
+        <v>101</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="3" ht="26.25" customHeight="1" s="4"/>
-    <row r="4" ht="26.25" customHeight="1" s="4"/>
-    <row r="5" ht="26.25" customHeight="1" s="4"/>
-    <row r="6" ht="26.25" customHeight="1" s="4"/>
-    <row r="7" ht="26.25" customHeight="1" s="4"/>
-    <row r="8" ht="26.25" customHeight="1" s="4"/>
-    <row r="9" ht="26.25" customHeight="1" s="4"/>
-    <row r="10" ht="27.75" customHeight="1" s="4"/>
-    <row r="11" ht="27.75" customHeight="1" s="4"/>
-    <row r="12" ht="27.75" customHeight="1" s="4"/>
-    <row r="13" ht="27.75" customHeight="1" s="4"/>
-    <row r="14" ht="27.75" customHeight="1" s="4"/>
-    <row r="15" ht="27.75" customHeight="1" s="4"/>
-    <row r="16" ht="27.75" customHeight="1" s="4"/>
-    <row r="17" ht="27.75" customHeight="1" s="4"/>
-    <row r="18" ht="27.75" customHeight="1" s="4"/>
-    <row r="19" ht="27.75" customHeight="1" s="4"/>
-    <row r="20" ht="27.75" customHeight="1" s="4"/>
-    <row r="21" ht="27.75" customHeight="1" s="4"/>
-    <row r="22" ht="27.75" customHeight="1" s="4"/>
-    <row r="23" ht="27.75" customHeight="1" s="4"/>
-    <row r="24" ht="27.75" customHeight="1" s="4"/>
-    <row r="25" ht="27.75" customHeight="1" s="4"/>
-    <row r="26" ht="27.75" customHeight="1" s="4"/>
-    <row r="27" ht="27.75" customHeight="1" s="4"/>
-    <row r="28" ht="27.75" customHeight="1" s="4"/>
-    <row r="29" ht="27.75" customHeight="1" s="4"/>
-    <row r="30" ht="27.75" customHeight="1" s="4"/>
-    <row r="31" ht="27.75" customHeight="1" s="4"/>
-    <row r="32" ht="27.75" customHeight="1" s="4"/>
-    <row r="33" ht="27.75" customHeight="1" s="4"/>
-    <row r="34" ht="27.75" customHeight="1" s="4"/>
-    <row r="35" ht="27.75" customHeight="1" s="4"/>
-    <row r="36" ht="27.75" customHeight="1" s="4"/>
-    <row r="37" ht="27.75" customHeight="1" s="4"/>
-    <row r="38" ht="27.75" customHeight="1" s="4"/>
-    <row r="39" ht="27.75" customHeight="1" s="4"/>
-    <row r="40" ht="27.75" customHeight="1" s="4"/>
-    <row r="41" ht="27.75" customHeight="1" s="4"/>
-    <row r="42" ht="27.75" customHeight="1" s="4"/>
-    <row r="43" ht="27.75" customHeight="1" s="4"/>
-    <row r="44" ht="27.75" customHeight="1" s="4"/>
-    <row r="45" ht="27.75" customHeight="1" s="4"/>
-    <row r="46" ht="27.75" customHeight="1" s="4"/>
-    <row r="47" ht="27.75" customHeight="1" s="4"/>
-    <row r="48" ht="13.8" customHeight="1" s="4"/>
-    <row r="49" ht="13.8" customHeight="1" s="4"/>
-    <row r="50" ht="13.8" customHeight="1" s="4"/>
-    <row r="51" ht="13.8" customHeight="1" s="4"/>
-    <row r="52" ht="13.8" customHeight="1" s="4"/>
-    <row r="53" ht="13.8" customHeight="1" s="4"/>
-    <row r="54" ht="13.8" customHeight="1" s="4"/>
-    <row r="55" ht="13.8" customHeight="1" s="4"/>
-    <row r="56" ht="13.8" customHeight="1" s="4"/>
-    <row r="57" ht="13.8" customHeight="1" s="4"/>
-    <row r="58" ht="13.8" customHeight="1" s="4"/>
-    <row r="59" ht="13.8" customHeight="1" s="4"/>
-    <row r="60" ht="13.8" customHeight="1" s="4"/>
-    <row r="61" ht="13.8" customHeight="1" s="4"/>
-    <row r="62" ht="13.8" customHeight="1" s="4"/>
-    <row r="63" ht="13.8" customHeight="1" s="4"/>
-    <row r="64" ht="13.8" customHeight="1" s="4"/>
-    <row r="65" ht="13.8" customHeight="1" s="4"/>
-    <row r="66" ht="13.8" customHeight="1" s="4"/>
-    <row r="67" ht="13.8" customHeight="1" s="4"/>
-    <row r="68" ht="13.8" customHeight="1" s="4"/>
-    <row r="69" ht="13.8" customHeight="1" s="4"/>
-    <row r="70" ht="13.8" customHeight="1" s="4"/>
-    <row r="71" ht="13.8" customHeight="1" s="4"/>
-    <row r="72" ht="13.8" customHeight="1" s="4"/>
-    <row r="73" ht="13.8" customHeight="1" s="4"/>
-    <row r="74" ht="13.8" customHeight="1" s="4"/>
-    <row r="75" ht="13.8" customHeight="1" s="4"/>
+    <row r="3" spans="1:8" ht="26.25" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="4">
+        <v>226000</v>
+      </c>
+      <c r="D3" s="5">
+        <v>41616</v>
+      </c>
+      <c r="E3" s="5">
+        <v>41619</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="4">
+        <v>102</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="26.25" customHeight="1">
+      <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="4">
+        <v>10000</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="4">
+        <v>103</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="26.25" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="4">
+        <v>77000</v>
+      </c>
+      <c r="D5" s="5">
+        <v>44198</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="6">
+        <v>104</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="26.25" customHeight="1">
+      <c r="A6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4">
+        <v>12000</v>
+      </c>
+      <c r="D6" s="5">
+        <v>44531</v>
+      </c>
+      <c r="E6" s="5">
+        <v>44533</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="6">
+        <v>105</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="26.25" customHeight="1"/>
+    <row r="8" spans="1:8" ht="26.25" customHeight="1"/>
+    <row r="9" spans="1:8" ht="26.25" customHeight="1"/>
+    <row r="10" spans="1:8" ht="27.75" customHeight="1"/>
+    <row r="11" spans="1:8" ht="27.75" customHeight="1"/>
+    <row r="12" spans="1:8" ht="27.75" customHeight="1"/>
+    <row r="13" spans="1:8" ht="27.75" customHeight="1"/>
+    <row r="14" spans="1:8" ht="27.75" customHeight="1"/>
+    <row r="15" spans="1:8" ht="27.75" customHeight="1"/>
+    <row r="16" spans="1:8" ht="27.75" customHeight="1"/>
+    <row r="17" ht="27.75" customHeight="1"/>
+    <row r="18" ht="27.75" customHeight="1"/>
+    <row r="19" ht="27.75" customHeight="1"/>
+    <row r="20" ht="27.75" customHeight="1"/>
+    <row r="21" ht="27.75" customHeight="1"/>
+    <row r="22" ht="27.75" customHeight="1"/>
+    <row r="23" ht="27.75" customHeight="1"/>
+    <row r="24" ht="27.75" customHeight="1"/>
+    <row r="25" ht="27.75" customHeight="1"/>
+    <row r="26" ht="27.75" customHeight="1"/>
+    <row r="27" ht="27.75" customHeight="1"/>
+    <row r="28" ht="27.75" customHeight="1"/>
+    <row r="29" ht="27.75" customHeight="1"/>
+    <row r="30" ht="27.75" customHeight="1"/>
+    <row r="31" ht="27.75" customHeight="1"/>
+    <row r="32" ht="27.75" customHeight="1"/>
+    <row r="33" ht="27.75" customHeight="1"/>
+    <row r="34" ht="27.75" customHeight="1"/>
+    <row r="35" ht="27.75" customHeight="1"/>
+    <row r="36" ht="27.75" customHeight="1"/>
+    <row r="37" ht="27.75" customHeight="1"/>
+    <row r="38" ht="27.75" customHeight="1"/>
+    <row r="39" ht="27.75" customHeight="1"/>
+    <row r="40" ht="27.75" customHeight="1"/>
+    <row r="41" ht="27.75" customHeight="1"/>
+    <row r="42" ht="27.75" customHeight="1"/>
+    <row r="43" ht="27.75" customHeight="1"/>
+    <row r="44" ht="27.75" customHeight="1"/>
+    <row r="45" ht="27.75" customHeight="1"/>
+    <row r="46" ht="27.75" customHeight="1"/>
+    <row r="47" ht="27.75" customHeight="1"/>
+    <row r="48" ht="13.9" customHeight="1"/>
+    <row r="49" ht="13.9" customHeight="1"/>
+    <row r="50" ht="13.9" customHeight="1"/>
+    <row r="51" ht="13.9" customHeight="1"/>
+    <row r="52" ht="13.9" customHeight="1"/>
+    <row r="53" ht="13.9" customHeight="1"/>
+    <row r="54" ht="13.9" customHeight="1"/>
+    <row r="55" ht="13.9" customHeight="1"/>
+    <row r="56" ht="13.9" customHeight="1"/>
+    <row r="57" ht="13.9" customHeight="1"/>
+    <row r="58" ht="13.9" customHeight="1"/>
+    <row r="59" ht="13.9" customHeight="1"/>
+    <row r="60" ht="13.9" customHeight="1"/>
+    <row r="61" ht="13.9" customHeight="1"/>
+    <row r="62" ht="13.9" customHeight="1"/>
+    <row r="63" ht="13.9" customHeight="1"/>
+    <row r="64" ht="13.9" customHeight="1"/>
+    <row r="65" ht="13.9" customHeight="1"/>
+    <row r="66" ht="13.9" customHeight="1"/>
+    <row r="67" ht="13.9" customHeight="1"/>
+    <row r="68" ht="13.9" customHeight="1"/>
+    <row r="69" ht="13.9" customHeight="1"/>
+    <row r="70" ht="13.9" customHeight="1"/>
+    <row r="71" ht="13.9" customHeight="1"/>
+    <row r="72" ht="13.9" customHeight="1"/>
+    <row r="73" ht="13.9" customHeight="1"/>
+    <row r="74" ht="13.9" customHeight="1"/>
+    <row r="75" ht="13.9" customHeight="1"/>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.9840277777777779" bottom="0.9840277777777779" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H4" r:id="rId3"/>
+    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="H6" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
creat and view function is working __normal case
</commit_message>
<xml_diff>
--- a/projects_data.xlsx
+++ b/projects_data.xlsx
@@ -1,146 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" iterateDelta="0.0001"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
-  <si>
-    <t>project title</t>
-  </si>
-  <si>
-    <t>Details</t>
-  </si>
-  <si>
-    <t>Total target</t>
-  </si>
-  <si>
-    <t>Start date</t>
-  </si>
-  <si>
-    <t>End date</t>
-  </si>
-  <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>omar</t>
-  </si>
-  <si>
-    <t>user_id</t>
-  </si>
-  <si>
-    <t>first project</t>
-  </si>
-  <si>
-    <t>start funding for school</t>
-  </si>
-  <si>
-    <t>22/7/2010</t>
-  </si>
-  <si>
-    <t>22/8/2010</t>
-  </si>
-  <si>
-    <t>mostafa</t>
-  </si>
-  <si>
-    <t>nour</t>
-  </si>
-  <si>
-    <t>mahmoud</t>
-  </si>
-  <si>
-    <t>22/9/2021</t>
-  </si>
-  <si>
-    <t>22/12/2021</t>
-  </si>
-  <si>
-    <t>30/3/2021</t>
-  </si>
-  <si>
-    <t>crtical surgary</t>
-  </si>
-  <si>
-    <t>new iphone</t>
-  </si>
-  <si>
-    <t>gaming set</t>
-  </si>
-  <si>
-    <t>weekend at hawaii</t>
-  </si>
-  <si>
-    <t>second project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">third project </t>
-  </si>
-  <si>
-    <t>fourth project</t>
-  </si>
-  <si>
-    <t>fifth project</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>abc_cd@ed.com</t>
-  </si>
-  <si>
-    <t>cd_ed@ed.com</t>
-  </si>
-  <si>
-    <t>xyz_as@ed.com</t>
-  </si>
-  <si>
-    <t>af_o@ed.com</t>
-  </si>
-  <si>
-    <t>wtf@ed.com</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="1"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="15"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
       <name val="Arial"/>
       <charset val="1"/>
+      <color theme="10"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -189,39 +89,38 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
-      <protection locked="0"/>
+      <protection locked="0" hidden="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -578,249 +477,345 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMK75"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" style="1" customWidth="1"/>
-    <col min="7" max="1025" width="14.42578125" style="1" customWidth="1"/>
+    <col width="24.5703125" customWidth="1" style="1" min="1" max="1"/>
+    <col width="48.140625" customWidth="1" style="1" min="2" max="2"/>
+    <col width="21.85546875" customWidth="1" style="1" min="3" max="3"/>
+    <col width="18.7109375" customWidth="1" style="1" min="4" max="4"/>
+    <col width="21.7109375" customWidth="1" style="1" min="5" max="5"/>
+    <col width="28.7109375" customWidth="1" style="1" min="6" max="6"/>
+    <col width="14.42578125" customWidth="1" style="1" min="7" max="1025"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="35.25" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>26</v>
+    <row r="1" ht="35.25" customHeight="1" s="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>project title</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Details</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Total target</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Start date</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>End date</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Owner</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>user_id</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4">
+    <row r="2" ht="26.25" customHeight="1" s="1">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>first project</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>start funding for school</t>
+        </is>
+      </c>
+      <c r="C2" s="6" t="n">
         <v>2500</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="4">
+      <c r="D2" s="6" t="inlineStr">
+        <is>
+          <t>22/7/2010</t>
+        </is>
+      </c>
+      <c r="E2" s="6" t="inlineStr">
+        <is>
+          <t>22/8/2010</t>
+        </is>
+      </c>
+      <c r="F2" s="6" t="inlineStr">
+        <is>
+          <t>omar</t>
+        </is>
+      </c>
+      <c r="G2" s="6" t="n">
         <v>101</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>27</v>
+      <c r="H2" s="7" t="inlineStr">
+        <is>
+          <t>abc_cd@ed.com</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="4">
+    <row r="3" ht="26.25" customHeight="1" s="1">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>second project</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>crtical surgary</t>
+        </is>
+      </c>
+      <c r="C3" s="6" t="n">
         <v>226000</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="5" t="n">
         <v>41616</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="5" t="n">
         <v>41619</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="4">
+      <c r="F3" s="6" t="inlineStr">
+        <is>
+          <t>omar</t>
+        </is>
+      </c>
+      <c r="G3" s="6" t="n">
         <v>102</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>28</v>
+      <c r="H3" s="8" t="inlineStr">
+        <is>
+          <t>cd_ed@ed.com</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="4">
+    <row r="4" ht="26.25" customHeight="1" s="1">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">third project </t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>new iphone</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="n">
         <v>10000</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="4">
+      <c r="D4" s="6" t="inlineStr">
+        <is>
+          <t>22/9/2021</t>
+        </is>
+      </c>
+      <c r="E4" s="6" t="inlineStr">
+        <is>
+          <t>22/12/2021</t>
+        </is>
+      </c>
+      <c r="F4" s="6" t="inlineStr">
+        <is>
+          <t>mostafa</t>
+        </is>
+      </c>
+      <c r="G4" s="6" t="n">
         <v>103</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>29</v>
+      <c r="H4" s="7" t="inlineStr">
+        <is>
+          <t>xyz_as@ed.com</t>
+        </is>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="4">
+    <row r="5" ht="26.25" customHeight="1" s="1">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>fourth project</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>gaming set</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="n">
         <v>77000</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="5" t="n">
         <v>44198</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="6">
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>30/3/2021</t>
+        </is>
+      </c>
+      <c r="F5" s="6" t="inlineStr">
+        <is>
+          <t>nour</t>
+        </is>
+      </c>
+      <c r="G5" s="6" t="n">
         <v>104</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>30</v>
+      <c r="H5" s="8" t="inlineStr">
+        <is>
+          <t>af_o@ed.com</t>
+        </is>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="4">
+    <row r="6" ht="26.25" customHeight="1" s="1">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>fifth project</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>weekend at hawaii</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="n">
         <v>12000</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="5" t="n">
         <v>44531</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="5" t="n">
         <v>44533</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="6">
+      <c r="F6" s="6" t="inlineStr">
+        <is>
+          <t>mahmoud</t>
+        </is>
+      </c>
+      <c r="G6" s="6" t="n">
         <v>105</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>31</v>
+      <c r="H6" s="8" t="inlineStr">
+        <is>
+          <t>wtf@ed.com</t>
+        </is>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="26.25" customHeight="1"/>
-    <row r="8" spans="1:8" ht="26.25" customHeight="1"/>
-    <row r="9" spans="1:8" ht="26.25" customHeight="1"/>
-    <row r="10" spans="1:8" ht="27.75" customHeight="1"/>
-    <row r="11" spans="1:8" ht="27.75" customHeight="1"/>
-    <row r="12" spans="1:8" ht="27.75" customHeight="1"/>
-    <row r="13" spans="1:8" ht="27.75" customHeight="1"/>
-    <row r="14" spans="1:8" ht="27.75" customHeight="1"/>
-    <row r="15" spans="1:8" ht="27.75" customHeight="1"/>
-    <row r="16" spans="1:8" ht="27.75" customHeight="1"/>
-    <row r="17" ht="27.75" customHeight="1"/>
-    <row r="18" ht="27.75" customHeight="1"/>
-    <row r="19" ht="27.75" customHeight="1"/>
-    <row r="20" ht="27.75" customHeight="1"/>
-    <row r="21" ht="27.75" customHeight="1"/>
-    <row r="22" ht="27.75" customHeight="1"/>
-    <row r="23" ht="27.75" customHeight="1"/>
-    <row r="24" ht="27.75" customHeight="1"/>
-    <row r="25" ht="27.75" customHeight="1"/>
-    <row r="26" ht="27.75" customHeight="1"/>
-    <row r="27" ht="27.75" customHeight="1"/>
-    <row r="28" ht="27.75" customHeight="1"/>
-    <row r="29" ht="27.75" customHeight="1"/>
-    <row r="30" ht="27.75" customHeight="1"/>
-    <row r="31" ht="27.75" customHeight="1"/>
-    <row r="32" ht="27.75" customHeight="1"/>
-    <row r="33" ht="27.75" customHeight="1"/>
-    <row r="34" ht="27.75" customHeight="1"/>
-    <row r="35" ht="27.75" customHeight="1"/>
-    <row r="36" ht="27.75" customHeight="1"/>
-    <row r="37" ht="27.75" customHeight="1"/>
-    <row r="38" ht="27.75" customHeight="1"/>
-    <row r="39" ht="27.75" customHeight="1"/>
-    <row r="40" ht="27.75" customHeight="1"/>
-    <row r="41" ht="27.75" customHeight="1"/>
-    <row r="42" ht="27.75" customHeight="1"/>
-    <row r="43" ht="27.75" customHeight="1"/>
-    <row r="44" ht="27.75" customHeight="1"/>
-    <row r="45" ht="27.75" customHeight="1"/>
-    <row r="46" ht="27.75" customHeight="1"/>
-    <row r="47" ht="27.75" customHeight="1"/>
-    <row r="48" ht="13.9" customHeight="1"/>
-    <row r="49" ht="13.9" customHeight="1"/>
-    <row r="50" ht="13.9" customHeight="1"/>
-    <row r="51" ht="13.9" customHeight="1"/>
-    <row r="52" ht="13.9" customHeight="1"/>
-    <row r="53" ht="13.9" customHeight="1"/>
-    <row r="54" ht="13.9" customHeight="1"/>
-    <row r="55" ht="13.9" customHeight="1"/>
-    <row r="56" ht="13.9" customHeight="1"/>
-    <row r="57" ht="13.9" customHeight="1"/>
-    <row r="58" ht="13.9" customHeight="1"/>
-    <row r="59" ht="13.9" customHeight="1"/>
-    <row r="60" ht="13.9" customHeight="1"/>
-    <row r="61" ht="13.9" customHeight="1"/>
-    <row r="62" ht="13.9" customHeight="1"/>
-    <row r="63" ht="13.9" customHeight="1"/>
-    <row r="64" ht="13.9" customHeight="1"/>
-    <row r="65" ht="13.9" customHeight="1"/>
-    <row r="66" ht="13.9" customHeight="1"/>
-    <row r="67" ht="13.9" customHeight="1"/>
-    <row r="68" ht="13.9" customHeight="1"/>
-    <row r="69" ht="13.9" customHeight="1"/>
-    <row r="70" ht="13.9" customHeight="1"/>
-    <row r="71" ht="13.9" customHeight="1"/>
-    <row r="72" ht="13.9" customHeight="1"/>
-    <row r="73" ht="13.9" customHeight="1"/>
-    <row r="74" ht="13.9" customHeight="1"/>
-    <row r="75" ht="13.9" customHeight="1"/>
+    <row r="7" ht="26.25" customHeight="1" s="1">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>this is a test creation</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>12000</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>12/8/2021</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>12/9/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="26.25" customHeight="1" s="1"/>
+    <row r="9" ht="26.25" customHeight="1" s="1"/>
+    <row r="10" ht="27.75" customHeight="1" s="1"/>
+    <row r="11" ht="27.75" customHeight="1" s="1"/>
+    <row r="12" ht="27.75" customHeight="1" s="1"/>
+    <row r="13" ht="27.75" customHeight="1" s="1"/>
+    <row r="14" ht="27.75" customHeight="1" s="1"/>
+    <row r="15" ht="27.75" customHeight="1" s="1"/>
+    <row r="16" ht="27.75" customHeight="1" s="1"/>
+    <row r="17" ht="27.75" customHeight="1" s="1"/>
+    <row r="18" ht="27.75" customHeight="1" s="1"/>
+    <row r="19" ht="27.75" customHeight="1" s="1"/>
+    <row r="20" ht="27.75" customHeight="1" s="1"/>
+    <row r="21" ht="27.75" customHeight="1" s="1"/>
+    <row r="22" ht="27.75" customHeight="1" s="1"/>
+    <row r="23" ht="27.75" customHeight="1" s="1"/>
+    <row r="24" ht="27.75" customHeight="1" s="1"/>
+    <row r="25" ht="27.75" customHeight="1" s="1"/>
+    <row r="26" ht="27.75" customHeight="1" s="1"/>
+    <row r="27" ht="27.75" customHeight="1" s="1"/>
+    <row r="28" ht="27.75" customHeight="1" s="1"/>
+    <row r="29" ht="27.75" customHeight="1" s="1"/>
+    <row r="30" ht="27.75" customHeight="1" s="1"/>
+    <row r="31" ht="27.75" customHeight="1" s="1"/>
+    <row r="32" ht="27.75" customHeight="1" s="1"/>
+    <row r="33" ht="27.75" customHeight="1" s="1"/>
+    <row r="34" ht="27.75" customHeight="1" s="1"/>
+    <row r="35" ht="27.75" customHeight="1" s="1"/>
+    <row r="36" ht="27.75" customHeight="1" s="1"/>
+    <row r="37" ht="27.75" customHeight="1" s="1"/>
+    <row r="38" ht="27.75" customHeight="1" s="1"/>
+    <row r="39" ht="27.75" customHeight="1" s="1"/>
+    <row r="40" ht="27.75" customHeight="1" s="1"/>
+    <row r="41" ht="27.75" customHeight="1" s="1"/>
+    <row r="42" ht="27.75" customHeight="1" s="1"/>
+    <row r="43" ht="27.75" customHeight="1" s="1"/>
+    <row r="44" ht="27.75" customHeight="1" s="1"/>
+    <row r="45" ht="27.75" customHeight="1" s="1"/>
+    <row r="46" ht="27.75" customHeight="1" s="1"/>
+    <row r="47" ht="27.75" customHeight="1" s="1"/>
+    <row r="48" ht="13.9" customHeight="1" s="1"/>
+    <row r="49" ht="13.9" customHeight="1" s="1"/>
+    <row r="50" ht="13.9" customHeight="1" s="1"/>
+    <row r="51" ht="13.9" customHeight="1" s="1"/>
+    <row r="52" ht="13.9" customHeight="1" s="1"/>
+    <row r="53" ht="13.9" customHeight="1" s="1"/>
+    <row r="54" ht="13.9" customHeight="1" s="1"/>
+    <row r="55" ht="13.9" customHeight="1" s="1"/>
+    <row r="56" ht="13.9" customHeight="1" s="1"/>
+    <row r="57" ht="13.9" customHeight="1" s="1"/>
+    <row r="58" ht="13.9" customHeight="1" s="1"/>
+    <row r="59" ht="13.9" customHeight="1" s="1"/>
+    <row r="60" ht="13.9" customHeight="1" s="1"/>
+    <row r="61" ht="13.9" customHeight="1" s="1"/>
+    <row r="62" ht="13.9" customHeight="1" s="1"/>
+    <row r="63" ht="13.9" customHeight="1" s="1"/>
+    <row r="64" ht="13.9" customHeight="1" s="1"/>
+    <row r="65" ht="13.9" customHeight="1" s="1"/>
+    <row r="66" ht="13.9" customHeight="1" s="1"/>
+    <row r="67" ht="13.9" customHeight="1" s="1"/>
+    <row r="68" ht="13.9" customHeight="1" s="1"/>
+    <row r="69" ht="13.9" customHeight="1" s="1"/>
+    <row r="70" ht="13.9" customHeight="1" s="1"/>
+    <row r="71" ht="13.9" customHeight="1" s="1"/>
+    <row r="72" ht="13.9" customHeight="1" s="1"/>
+    <row r="73" ht="13.9" customHeight="1" s="1"/>
+    <row r="74" ht="13.9" customHeight="1" s="1"/>
+    <row r="75" ht="13.9" customHeight="1" s="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1"/>
@@ -829,7 +824,7 @@
     <hyperlink ref="H5" r:id="rId4"/>
     <hyperlink ref="H6" r:id="rId5"/>
   </hyperlinks>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.9840277777777779" bottom="0.9840277777777779" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" firstPageNumber="0" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
trying to refactor #1
</commit_message>
<xml_diff>
--- a/projects_data.xlsx
+++ b/projects_data.xlsx
@@ -711,27 +711,27 @@
     <row r="8" ht="26.25" customHeight="1" s="4">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>after edit</t>
+          <t>project 2</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>after edit is done</t>
+          <t>edited</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>111</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>13/8/2021</t>
+          <t>11/8/2021</t>
         </is>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>13/9/2021</t>
+          <t>12/8/2021</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
@@ -743,17 +743,17 @@
     <row r="9" ht="26.25" customHeight="1" s="4">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>peoject2</t>
+          <t>test 4</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>test 2</t>
+          <t>1111</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>111</t>
+          <t>1111</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
@@ -763,7 +763,7 @@
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>12/8/2021</t>
+          <t>11/9/2021</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
@@ -775,17 +775,17 @@
     <row r="10" ht="27.75" customHeight="1" s="4">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>project3</t>
+          <t>project 5</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>test3</t>
+          <t>test5</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>121</t>
+          <t>1223</t>
         </is>
       </c>
       <c r="D10" s="3" t="inlineStr">
@@ -795,7 +795,7 @@
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>10/9/2021</t>
+          <t>11/10/2021</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
@@ -807,27 +807,27 @@
     <row r="11" ht="27.75" customHeight="1" s="4">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>project4</t>
+          <t>final</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>test4</t>
+          <t>test final</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>1111</t>
+          <t>9998</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>17/8/2021</t>
+          <t>11/8/2021</t>
         </is>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>11/9/2021</t>
+          <t>10/11/2021</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">

</xml_diff>